<commit_message>
update dashboard, add vote_date and attend on event_hub
</commit_message>
<xml_diff>
--- a/db/uploads/50gacoopb2.xlsx
+++ b/db/uploads/50gacoopb2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansellgabrieldelayre/Sites/GA_system/db/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BE053D-A4FF-6F4F-BD6D-988DBE59C6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9988B8CA-BD21-AC49-B9DC-CC28DAF6B1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="1140" windowWidth="27640" windowHeight="16940" xr2:uid="{4088DED9-C2FE-0443-8663-EB22148B5F7E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="1827">
   <si>
     <t>6681 DEVELOPMENT COOPERATIVE</t>
   </si>
@@ -5489,6 +5489,33 @@
   </si>
   <si>
     <t>LKP6</t>
+  </si>
+  <si>
+    <t>Naga School Teachers Multipurpose Cooperative</t>
+  </si>
+  <si>
+    <t>AGA00617</t>
+  </si>
+  <si>
+    <t>Maasin Community Multipurpose Cooperative</t>
+  </si>
+  <si>
+    <t>AGA00618</t>
+  </si>
+  <si>
+    <t>Cebu City Public School Teachers and Employees Multipurpose Cooperative</t>
+  </si>
+  <si>
+    <t>AGA00619</t>
+  </si>
+  <si>
+    <t>KDDF</t>
+  </si>
+  <si>
+    <t>RLRH</t>
+  </si>
+  <si>
+    <t>RD2U</t>
   </si>
 </sst>
 </file>
@@ -6024,10 +6051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0FCE4F-CA76-5849-AD49-C504473696A2}">
-  <dimension ref="A2:D610"/>
+  <dimension ref="A2:D613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A596" workbookViewId="0">
-      <selection activeCell="A604" sqref="A604"/>
+    <sheetView tabSelected="1" topLeftCell="A585" workbookViewId="0">
+      <selection activeCell="C612" sqref="C612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12719,7 +12746,40 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="610" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="610" spans="1:3" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A610" s="20" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B610" s="18" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C610" s="19" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A611" s="20" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B611" s="18" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C611" s="19" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="612" spans="1:3" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A612" s="20" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B612" s="18" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C612" s="19" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>